<commit_message>
RETC_062 and RETC_063 upload
</commit_message>
<xml_diff>
--- a/final-framework-testng/documents/Testdata.xlsx
+++ b/final-framework-testng/documents/Testdata.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095A6636-C6AD-453F-BDF0-7F91485A60D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC70EFFE-4EC7-49FA-9CB5-F7F358E0AA21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>manzoor@gmail.com</t>
   </si>
@@ -38,6 +39,18 @@
   </si>
   <si>
     <t>mariya</t>
+  </si>
+  <si>
+    <t>manzoor</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -401,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -452,4 +465,72 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DB7511-B47B-44BD-91FD-29179D04A828}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>76576</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>876876</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3919F2FB-728B-4578-B023-C99ADD46614E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3DA7E071-34C0-4B50-83F1-0AA5FAF43461}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{FCD5924E-654B-4767-AB02-23109C9D505F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>